<commit_message>
AIP-2106 AIP-2110 Code commited for Double partial cabling adjustnment
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/RMS_Data_Validation_Cablings/1U1U3I3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/RMS_Data_Validation_Cablings/1U1U3I3I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6A3FBA-A3E4-4B7B-891E-80FB20B23DA9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2AEF64-C1E8-487F-9D1F-CD2B7C9DB320}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
   <si>
     <t>Channel</t>
   </si>
@@ -177,12 +177,6 @@
   </si>
   <si>
     <t>Channel[13]</t>
-  </si>
-  <si>
-    <t>Channel[14]</t>
-  </si>
-  <si>
-    <t>Channel[15]</t>
   </si>
   <si>
     <t>UNIT</t>
@@ -742,18 +736,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -815,13 +809,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
         <v>55</v>
-      </c>
-      <c r="K1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -835,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -853,13 +847,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -873,13 +867,13 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
@@ -891,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -905,13 +899,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -923,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -937,13 +931,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>18</v>
@@ -955,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -969,7 +963,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -987,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W6" t="s">
         <v>19</v>
@@ -1005,7 +999,7 @@
         <v>15</v>
       </c>
       <c r="AB6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1019,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -1037,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -1049,13 +1043,13 @@
         <v>11</v>
       </c>
       <c r="Z7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA7" t="s">
         <v>16</v>
       </c>
       <c r="AB7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1069,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -1087,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W8" t="s">
         <v>21</v>
@@ -1096,13 +1090,13 @@
         <v>12</v>
       </c>
       <c r="Z8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AA8" t="s">
         <v>17</v>
       </c>
       <c r="AB8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -1116,13 +1110,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>15</v>
@@ -1134,22 +1128,22 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W9" t="s">
         <v>22</v>
       </c>
       <c r="Y9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA9" t="s">
         <v>66</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AB9" t="s">
         <v>67</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1163,13 +1157,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>16</v>
@@ -1181,22 +1175,22 @@
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W10" t="s">
         <v>23</v>
       </c>
       <c r="Y10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA10" t="s">
         <v>18</v>
       </c>
       <c r="AB10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1210,13 +1204,13 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>15</v>
@@ -1228,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W11" t="s">
         <v>24</v>
       </c>
       <c r="Y11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1248,13 +1242,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>18</v>
@@ -1266,7 +1260,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W12" t="s">
         <v>25</v>
@@ -1283,13 +1277,13 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>18</v>
@@ -1301,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W13" t="s">
         <v>26</v>
@@ -1318,13 +1312,13 @@
         <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>17</v>
@@ -1336,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W14" t="s">
         <v>27</v>
@@ -1353,13 +1347,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>18</v>
@@ -1371,78 +1365,38 @@
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="W16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="W17" t="s">
         <v>30</v>
       </c>
@@ -1536,15 +1490,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1552,7 +1506,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -1560,7 +1514,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1568,7 +1522,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1576,15 +1530,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" s="2">
-        <v>4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2">
         <v>-1</v>
@@ -1601,7 +1555,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,15 +1565,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1627,7 +1581,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -1635,7 +1589,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1643,7 +1597,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1651,7 +1605,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -1659,7 +1613,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -1667,7 +1621,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1675,7 +1629,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1683,7 +1637,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1691,7 +1645,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -1699,7 +1653,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -1707,7 +1661,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
@@ -1715,7 +1669,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1">
         <v>7</v>
@@ -1723,7 +1677,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -1731,7 +1685,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -1739,7 +1693,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1747,7 +1701,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -1755,7 +1709,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -1763,7 +1717,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20">
         <v>13</v>
@@ -1771,7 +1725,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1779,7 +1733,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1787,7 +1741,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1795,7 +1749,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1803,7 +1757,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1811,7 +1765,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -1819,7 +1773,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1827,7 +1781,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1835,7 +1789,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1843,7 +1797,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B30">
         <v>11</v>
@@ -1851,7 +1805,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B31">
         <v>12</v>
@@ -1859,7 +1813,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>14</v>
@@ -1867,7 +1821,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1875,7 +1829,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1883,7 +1837,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1891,23 +1845,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1915,7 +1869,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1923,15 +1877,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1961,16 +1915,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,7 +2036,7 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>